<commit_message>
learning page, loading page and style updates
</commit_message>
<xml_diff>
--- a/data/fakeleaderboard.xlsx
+++ b/data/fakeleaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny\OneDrive - ort braude college of engineering\טכנולוגיות WEB\project repo\B6\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB47E9D-13D3-4508-B4EE-FB4B86025721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2299A6-C3CA-4291-953E-23211761402F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31530" yWindow="7035" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,72 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>Bitcoin</t>
-  </si>
-  <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>Ethereum</t>
-  </si>
-  <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>Cardano</t>
-  </si>
-  <si>
-    <t>ADA</t>
-  </si>
-  <si>
-    <t>Binance Coin</t>
-  </si>
-  <si>
-    <t>BNB</t>
-  </si>
-  <si>
-    <t>Solana</t>
-  </si>
-  <si>
-    <t>SOL</t>
-  </si>
-  <si>
-    <t>XRP</t>
-  </si>
-  <si>
-    <t>Polkadot</t>
-  </si>
-  <si>
-    <t>DOT</t>
-  </si>
-  <si>
-    <t>Dogecoin</t>
-  </si>
-  <si>
-    <t>DOGE</t>
-  </si>
-  <si>
-    <t>Chainlink</t>
-  </si>
-  <si>
-    <t>LINK</t>
-  </si>
-  <si>
-    <t>Litecoin</t>
-  </si>
-  <si>
-    <t>LTC</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Score</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Shimron</t>
+  </si>
+  <si>
+    <t>Roi</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Bill Gates</t>
+  </si>
+  <si>
+    <t>Elon Mask</t>
+  </si>
+  <si>
+    <t>Mark Zuckerberg</t>
+  </si>
+  <si>
+    <t>Jeff Bezos</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>Drake</t>
   </si>
 </sst>
 </file>
@@ -121,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,20 +402,20 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -449,10 +423,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,10 +434,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>11000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,10 +445,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,8 +458,8 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="C5">
+        <v>9000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,8 +469,8 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
+      <c r="C6">
+        <v>8000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,10 +478,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>7000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -515,10 +489,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>6000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -526,10 +500,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>5000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,10 +511,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,10 +522,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>-2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>